<commit_message>
Revert "Update workplan + report"
This reverts commit e7ff0c4fbc11eada4b5a72f9e87496093231e668.
</commit_message>
<xml_diff>
--- a/final-project-workload-final.xlsx
+++ b/final-project-workload-final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toma Volentir\Desktop\final_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TUD\Y2\CG\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3032F9E-A1E5-4893-9515-F532C6DC2B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB1DF2A-19CE-4687-A72C-59DBC9061B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -324,8 +324,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -340,13 +346,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -357,10 +363,10 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -376,6 +382,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -391,14 +400,8 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -786,13 +789,13 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="3" width="48.42578125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="48.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="21.140625" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" customWidth="1"/>
@@ -803,541 +806,541 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="29">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="32">
         <v>5467640</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="32">
         <v>5470668</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="32">
         <v>5454123</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="29" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="32" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="11">
         <v>0.5</v>
       </c>
-      <c r="D8" s="10">
-        <v>0</v>
-      </c>
-      <c r="E8" s="10">
-        <v>0</v>
-      </c>
-      <c r="F8" s="11">
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" ref="G8:G15" si="0">SUM(D8:F8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="15">
+        <v>1</v>
+      </c>
+      <c r="D10" s="12">
         <v>100</v>
       </c>
-      <c r="G8" s="5">
-        <f t="shared" ref="G8:G15" si="0">SUM(D8:F8)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="10">
-        <v>0</v>
-      </c>
-      <c r="E9" s="10">
-        <v>0</v>
-      </c>
-      <c r="F9" s="11">
-        <v>100</v>
-      </c>
-      <c r="G9" s="5">
+      <c r="E10" s="12">
+        <v>0</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="13">
-        <v>1</v>
-      </c>
-      <c r="D10" s="10">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="15">
+        <v>4</v>
+      </c>
+      <c r="D11" s="12">
         <v>100</v>
       </c>
-      <c r="E10" s="10">
-        <v>0</v>
-      </c>
-      <c r="F10" s="11">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5">
+      <c r="E11" s="12">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="13">
-        <v>4</v>
-      </c>
-      <c r="D11" s="10">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="17">
+        <v>5</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="17">
+        <v>3</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="17">
+        <v>1</v>
+      </c>
+      <c r="D14" s="12">
         <v>100</v>
       </c>
-      <c r="E11" s="10">
-        <v>0</v>
-      </c>
-      <c r="F11" s="11">
-        <v>0</v>
-      </c>
-      <c r="G11" s="5">
+      <c r="E14" s="12">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="15">
-        <v>5</v>
-      </c>
-      <c r="D12" s="10">
-        <v>0</v>
-      </c>
-      <c r="E12" s="10">
-        <v>0</v>
-      </c>
-      <c r="F12" s="11">
-        <v>0</v>
-      </c>
-      <c r="G12" s="5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0</v>
+      </c>
+      <c r="E15" s="12">
+        <v>0</v>
+      </c>
+      <c r="F15" s="13">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="15">
-        <v>3</v>
-      </c>
-      <c r="D13" s="10">
-        <v>0</v>
-      </c>
-      <c r="E13" s="10">
-        <v>0</v>
-      </c>
-      <c r="F13" s="11">
-        <v>100</v>
-      </c>
-      <c r="G13" s="5">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="15">
-        <v>1</v>
-      </c>
-      <c r="D14" s="10">
-        <v>100</v>
-      </c>
-      <c r="E14" s="10">
-        <v>0</v>
-      </c>
-      <c r="F14" s="11">
-        <v>0</v>
-      </c>
-      <c r="G14" s="5">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="15">
-        <v>1.5</v>
-      </c>
-      <c r="D15" s="10">
-        <v>0</v>
-      </c>
-      <c r="E15" s="10">
-        <v>0</v>
-      </c>
-      <c r="F15" s="11">
-        <v>33.33</v>
-      </c>
-      <c r="G15" s="5">
-        <f t="shared" si="0"/>
-        <v>33.33</v>
-      </c>
-    </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="20">
         <f>SUM(C8:C15)</f>
         <v>18</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="21">
         <f>SUMPRODUCT(C8:C15,D8:D15)/100</f>
         <v>6</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="21">
         <f>SUMPRODUCT($C8:$C15,E8:E15)/100</f>
         <v>0</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="21">
         <f>SUMPRODUCT($C8:$C15,F8:F15)/100</f>
-        <v>5.9999500000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="20" t="s">
+      <c r="A18" s="18"/>
+      <c r="B18" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="7" t="s">
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="8" t="s">
+      <c r="A19" s="18"/>
+      <c r="B19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="23">
         <v>1.5</v>
       </c>
-      <c r="D19" s="21">
-        <v>0</v>
-      </c>
-      <c r="E19" s="10">
-        <v>0</v>
-      </c>
-      <c r="F19" s="11">
-        <v>0</v>
-      </c>
-      <c r="G19" s="5">
+      <c r="D19" s="24">
+        <v>0</v>
+      </c>
+      <c r="E19" s="12">
+        <v>0</v>
+      </c>
+      <c r="F19" s="13">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7">
         <f t="shared" ref="G19:G28" si="1">SUM(D19:F19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="23">
         <v>1.5</v>
       </c>
-      <c r="D20" s="21">
-        <v>0</v>
-      </c>
-      <c r="E20" s="10">
-        <v>0</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0</v>
-      </c>
-      <c r="G20" s="5">
+      <c r="D20" s="24">
+        <v>0</v>
+      </c>
+      <c r="E20" s="12">
+        <v>0</v>
+      </c>
+      <c r="F20" s="13">
+        <v>0</v>
+      </c>
+      <c r="G20" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="23">
         <v>2.5</v>
       </c>
-      <c r="D21" s="21">
-        <v>0</v>
-      </c>
-      <c r="E21" s="10">
-        <v>0</v>
-      </c>
-      <c r="F21" s="11">
-        <v>0</v>
-      </c>
-      <c r="G21" s="5">
+      <c r="D21" s="24">
+        <v>0</v>
+      </c>
+      <c r="E21" s="12">
+        <v>0</v>
+      </c>
+      <c r="F21" s="13">
+        <v>0</v>
+      </c>
+      <c r="G21" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="23">
         <v>1.5</v>
       </c>
-      <c r="D22" s="21">
-        <v>0</v>
-      </c>
-      <c r="E22" s="10">
-        <v>0</v>
-      </c>
-      <c r="F22" s="11">
+      <c r="D22" s="24">
+        <v>0</v>
+      </c>
+      <c r="E22" s="12">
+        <v>0</v>
+      </c>
+      <c r="F22" s="13">
+        <v>0</v>
+      </c>
+      <c r="G22" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="24">
+        <v>0</v>
+      </c>
+      <c r="E23" s="12">
+        <v>0</v>
+      </c>
+      <c r="F23" s="13">
+        <v>0</v>
+      </c>
+      <c r="G23" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="23">
+        <v>2</v>
+      </c>
+      <c r="D24" s="24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="12">
+        <v>0</v>
+      </c>
+      <c r="F24" s="13">
+        <v>0</v>
+      </c>
+      <c r="G24" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="D25" s="24">
+        <v>0</v>
+      </c>
+      <c r="E25" s="12">
+        <v>0</v>
+      </c>
+      <c r="F25" s="13">
+        <v>0</v>
+      </c>
+      <c r="G25" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="23">
+        <v>2.5</v>
+      </c>
+      <c r="D26" s="24">
         <v>100</v>
       </c>
-      <c r="G22" s="5">
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="13">
+        <v>0</v>
+      </c>
+      <c r="G26" s="7">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="D23" s="21">
-        <v>0</v>
-      </c>
-      <c r="E23" s="10">
-        <v>0</v>
-      </c>
-      <c r="F23" s="11">
-        <v>0</v>
-      </c>
-      <c r="G23" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="9">
-        <v>2</v>
-      </c>
-      <c r="D24" s="21">
-        <v>0</v>
-      </c>
-      <c r="E24" s="10">
-        <v>0</v>
-      </c>
-      <c r="F24" s="11">
-        <v>0</v>
-      </c>
-      <c r="G24" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="9">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="23">
         <v>1.5</v>
       </c>
-      <c r="D25" s="21">
-        <v>0</v>
-      </c>
-      <c r="E25" s="10">
-        <v>0</v>
-      </c>
-      <c r="F25" s="11">
-        <v>0</v>
-      </c>
-      <c r="G25" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="D26" s="21">
+      <c r="D27" s="24">
         <v>100</v>
       </c>
-      <c r="E26" s="10">
-        <v>0</v>
-      </c>
-      <c r="F26" s="11">
-        <v>0</v>
-      </c>
-      <c r="G26" s="5">
+      <c r="E27" s="12">
+        <v>0</v>
+      </c>
+      <c r="F27" s="13">
+        <v>0</v>
+      </c>
+      <c r="G27" s="7">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="D27" s="21">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="23">
+        <v>3</v>
+      </c>
+      <c r="D28" s="24">
         <v>100</v>
       </c>
-      <c r="E27" s="10">
-        <v>0</v>
-      </c>
-      <c r="F27" s="11">
-        <v>0</v>
-      </c>
-      <c r="G27" s="5">
+      <c r="E28" s="12">
+        <v>0</v>
+      </c>
+      <c r="F28" s="13">
+        <v>0</v>
+      </c>
+      <c r="G28" s="7">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="9">
-        <v>3</v>
-      </c>
-      <c r="D28" s="21">
-        <v>100</v>
-      </c>
-      <c r="E28" s="10">
-        <v>0</v>
-      </c>
-      <c r="F28" s="11">
-        <v>0</v>
-      </c>
-      <c r="G28" s="5">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="23">
+      <c r="C29" s="26">
         <f>SUM(C19:C28)</f>
         <v>18</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="21">
         <f>SUMPRODUCT($C19:$C28,D19:D28)/100</f>
         <v>7</v>
       </c>
-      <c r="E29" s="19">
+      <c r="E29" s="21">
         <f>SUMPRODUCT($C19:$C28,E19:E28)/100</f>
         <v>0</v>
       </c>
-      <c r="F29" s="19">
+      <c r="F29" s="21">
         <f>SUMPRODUCT($C19:$C28,F19:F28)/100</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26">
+      <c r="C31" s="28"/>
+      <c r="D31" s="29">
         <f>D$16+D29</f>
         <v>13</v>
       </c>
-      <c r="E31" s="26">
+      <c r="E31" s="29">
         <f>E$16+E29</f>
         <v>0</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F31" s="30">
         <f>F$16+F29</f>
-        <v>7.4999500000000001</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1359,17 +1362,17 @@
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="31" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="31" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update workplan + report
</commit_message>
<xml_diff>
--- a/final-project-workload-final.xlsx
+++ b/final-project-workload-final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TUD\Y2\CG\final_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toma Volentir\Desktop\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB1DF2A-19CE-4687-A72C-59DBC9061B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3032F9E-A1E5-4893-9515-F532C6DC2B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -324,14 +324,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -346,13 +340,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -363,10 +357,10 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -382,9 +376,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -400,8 +391,14 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -789,13 +786,13 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="3" width="48.42578125" style="3" customWidth="1"/>
+    <col min="2" max="3" width="48.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" customWidth="1"/>
@@ -806,541 +803,541 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="3" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="32">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="29">
         <v>5467640</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="29">
         <v>5470668</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="29">
         <v>5454123</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="32" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>0.5</v>
       </c>
-      <c r="D8" s="12">
-        <v>0</v>
-      </c>
-      <c r="E8" s="12">
-        <v>0</v>
-      </c>
-      <c r="F8" s="13">
-        <v>0</v>
-      </c>
-      <c r="G8" s="7">
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11">
+        <v>100</v>
+      </c>
+      <c r="G8" s="5">
         <f t="shared" ref="G8:G15" si="0">SUM(D8:F8)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <v>2</v>
       </c>
-      <c r="D9" s="12">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12">
-        <v>0</v>
-      </c>
-      <c r="F9" s="13">
-        <v>0</v>
-      </c>
-      <c r="G9" s="7">
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
+        <v>100</v>
+      </c>
+      <c r="G9" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="13">
         <v>1</v>
       </c>
-      <c r="D10" s="12">
-        <v>100</v>
-      </c>
-      <c r="E10" s="12">
-        <v>0</v>
-      </c>
-      <c r="F10" s="13">
-        <v>0</v>
-      </c>
-      <c r="G10" s="7">
+      <c r="D10" s="10">
+        <v>100</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="13">
         <v>4</v>
       </c>
-      <c r="D11" s="12">
-        <v>100</v>
-      </c>
-      <c r="E11" s="12">
-        <v>0</v>
-      </c>
-      <c r="F11" s="13">
-        <v>0</v>
-      </c>
-      <c r="G11" s="7">
+      <c r="D11" s="10">
+        <v>100</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="15">
         <v>5</v>
       </c>
-      <c r="D12" s="12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="12">
-        <v>0</v>
-      </c>
-      <c r="F12" s="13">
-        <v>0</v>
-      </c>
-      <c r="G12" s="7">
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="15">
         <v>3</v>
       </c>
-      <c r="D13" s="12">
-        <v>0</v>
-      </c>
-      <c r="E13" s="12">
-        <v>0</v>
-      </c>
-      <c r="F13" s="13">
-        <v>0</v>
-      </c>
-      <c r="G13" s="7">
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11">
+        <v>100</v>
+      </c>
+      <c r="G13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="15">
         <v>1</v>
       </c>
-      <c r="D14" s="12">
-        <v>100</v>
-      </c>
-      <c r="E14" s="12">
-        <v>0</v>
-      </c>
-      <c r="F14" s="13">
-        <v>0</v>
-      </c>
-      <c r="G14" s="7">
+      <c r="D14" s="10">
+        <v>100</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="15">
         <v>1.5</v>
       </c>
-      <c r="D15" s="12">
-        <v>0</v>
-      </c>
-      <c r="E15" s="12">
-        <v>0</v>
-      </c>
-      <c r="F15" s="13">
-        <v>0</v>
-      </c>
-      <c r="G15" s="7">
+      <c r="D15" s="10">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>33.33</v>
+      </c>
+      <c r="G15" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="18">
         <f>SUM(C8:C15)</f>
         <v>18</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="19">
         <f>SUMPRODUCT(C8:C15,D8:D15)/100</f>
         <v>6</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="19">
         <f>SUMPRODUCT($C8:$C15,E8:E15)/100</f>
         <v>0</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="19">
         <f>SUMPRODUCT($C8:$C15,F8:F15)/100</f>
-        <v>0</v>
+        <v>5.9999500000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="22" t="s">
+      <c r="A18" s="16"/>
+      <c r="B18" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="10" t="s">
+      <c r="A19" s="16"/>
+      <c r="B19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="9">
         <v>1.5</v>
       </c>
-      <c r="D19" s="24">
-        <v>0</v>
-      </c>
-      <c r="E19" s="12">
-        <v>0</v>
-      </c>
-      <c r="F19" s="13">
-        <v>0</v>
-      </c>
-      <c r="G19" s="7">
+      <c r="D19" s="21">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0</v>
+      </c>
+      <c r="F19" s="11">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5">
         <f t="shared" ref="G19:G28" si="1">SUM(D19:F19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="9">
         <v>1.5</v>
       </c>
-      <c r="D20" s="24">
-        <v>0</v>
-      </c>
-      <c r="E20" s="12">
-        <v>0</v>
-      </c>
-      <c r="F20" s="13">
-        <v>0</v>
-      </c>
-      <c r="G20" s="7">
+      <c r="D20" s="21">
+        <v>0</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="23">
+      <c r="C21" s="9">
         <v>2.5</v>
       </c>
-      <c r="D21" s="24">
-        <v>0</v>
-      </c>
-      <c r="E21" s="12">
-        <v>0</v>
-      </c>
-      <c r="F21" s="13">
-        <v>0</v>
-      </c>
-      <c r="G21" s="7">
+      <c r="D21" s="21">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0</v>
+      </c>
+      <c r="F21" s="11">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="23">
+      <c r="C22" s="9">
         <v>1.5</v>
       </c>
-      <c r="D22" s="24">
-        <v>0</v>
-      </c>
-      <c r="E22" s="12">
-        <v>0</v>
-      </c>
-      <c r="F22" s="13">
-        <v>0</v>
-      </c>
-      <c r="G22" s="7">
+      <c r="D22" s="21">
+        <v>0</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0</v>
+      </c>
+      <c r="F22" s="11">
+        <v>100</v>
+      </c>
+      <c r="G22" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C23" s="9">
         <v>0.5</v>
       </c>
-      <c r="D23" s="24">
-        <v>0</v>
-      </c>
-      <c r="E23" s="12">
-        <v>0</v>
-      </c>
-      <c r="F23" s="13">
-        <v>0</v>
-      </c>
-      <c r="G23" s="7">
+      <c r="D23" s="21">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0</v>
+      </c>
+      <c r="F23" s="11">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="23">
+      <c r="C24" s="9">
         <v>2</v>
       </c>
-      <c r="D24" s="24">
-        <v>0</v>
-      </c>
-      <c r="E24" s="12">
-        <v>0</v>
-      </c>
-      <c r="F24" s="13">
-        <v>0</v>
-      </c>
-      <c r="G24" s="7">
+      <c r="D24" s="21">
+        <v>0</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0</v>
+      </c>
+      <c r="F24" s="11">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C25" s="9">
         <v>1.5</v>
       </c>
-      <c r="D25" s="24">
-        <v>0</v>
-      </c>
-      <c r="E25" s="12">
-        <v>0</v>
-      </c>
-      <c r="F25" s="13">
-        <v>0</v>
-      </c>
-      <c r="G25" s="7">
+      <c r="D25" s="21">
+        <v>0</v>
+      </c>
+      <c r="E25" s="10">
+        <v>0</v>
+      </c>
+      <c r="F25" s="11">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="23">
+      <c r="C26" s="9">
         <v>2.5</v>
       </c>
-      <c r="D26" s="24">
-        <v>100</v>
-      </c>
-      <c r="E26" s="12">
-        <v>0</v>
-      </c>
-      <c r="F26" s="13">
-        <v>0</v>
-      </c>
-      <c r="G26" s="7">
+      <c r="D26" s="21">
+        <v>100</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0</v>
+      </c>
+      <c r="F26" s="11">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C27" s="9">
         <v>1.5</v>
       </c>
-      <c r="D27" s="24">
-        <v>100</v>
-      </c>
-      <c r="E27" s="12">
-        <v>0</v>
-      </c>
-      <c r="F27" s="13">
-        <v>0</v>
-      </c>
-      <c r="G27" s="7">
+      <c r="D27" s="21">
+        <v>100</v>
+      </c>
+      <c r="E27" s="10">
+        <v>0</v>
+      </c>
+      <c r="F27" s="11">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="23">
+      <c r="C28" s="9">
         <v>3</v>
       </c>
-      <c r="D28" s="24">
-        <v>100</v>
-      </c>
-      <c r="E28" s="12">
-        <v>0</v>
-      </c>
-      <c r="F28" s="13">
-        <v>0</v>
-      </c>
-      <c r="G28" s="7">
+      <c r="D28" s="21">
+        <v>100</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0</v>
+      </c>
+      <c r="F28" s="11">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="23">
         <f>SUM(C19:C28)</f>
         <v>18</v>
       </c>
-      <c r="D29" s="21">
+      <c r="D29" s="19">
         <f>SUMPRODUCT($C19:$C28,D19:D28)/100</f>
         <v>7</v>
       </c>
-      <c r="E29" s="21">
+      <c r="E29" s="19">
         <f>SUMPRODUCT($C19:$C28,E19:E28)/100</f>
         <v>0</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F29" s="19">
         <f>SUMPRODUCT($C19:$C28,F19:F28)/100</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29">
+      <c r="C31" s="25"/>
+      <c r="D31" s="26">
         <f>D$16+D29</f>
         <v>13</v>
       </c>
-      <c r="E31" s="29">
+      <c r="E31" s="26">
         <f>E$16+E29</f>
         <v>0</v>
       </c>
-      <c r="F31" s="30">
+      <c r="F31" s="27">
         <f>F$16+F29</f>
-        <v>0</v>
+        <v>7.4999500000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1362,17 +1359,17 @@
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="28" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="28" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>